<commit_message>
Documento de pruebas actualizado
Documento de pruebas actualziado con la primera actualización del sprint
</commit_message>
<xml_diff>
--- a/Documentation/Diagnostico App.xlsx
+++ b/Documentation/Diagnostico App.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="62">
   <si>
     <t>Login</t>
   </si>
@@ -207,13 +207,16 @@
   </si>
   <si>
     <t>Entrega 1</t>
+  </si>
+  <si>
+    <t>El usuario debe conocer los codigos de los otros grupos?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +225,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -261,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -376,21 +387,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -399,6 +446,21 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -414,16 +476,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +774,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,610 +783,773 @@
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="2"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E4" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E5" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="E6" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E7" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E8" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="2"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E10" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E11" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="E12" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E13" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E14" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="6">
         <f>2/10</f>
         <v>0.2</v>
       </c>
-      <c r="D15" s="25"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="9">
+        <f>4/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="25" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="29"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26"/>
+      <c r="B20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <f>4/4</f>
         <v>1</v>
       </c>
-      <c r="D20" s="19"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="D20" s="12"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="29"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="18" t="s">
+      <c r="E22" s="32"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="24"/>
+      <c r="B23" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <f>2/2</f>
         <v>1</v>
       </c>
-      <c r="D23" s="19"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="D23" s="12"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="E24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="C27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
       <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="C28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" s="20" t="s">
+      <c r="C29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="24"/>
+      <c r="B30" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="8">
         <f>5/6</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="D30" s="23"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="D30" s="30"/>
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="28"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
       <c r="B32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
-      <c r="B33" s="21" t="s">
+      <c r="E32" s="35"/>
+      <c r="F32" s="36"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="24"/>
+      <c r="B33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="9">
         <f>1/2</f>
         <v>0.5</v>
       </c>
-      <c r="D33" s="22"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="D33" s="15"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="29"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
       <c r="B35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+      <c r="E35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
       <c r="B36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="E36" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
       <c r="B37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="E37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
       <c r="B38" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="26" t="s">
+      <c r="E38" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="23"/>
+      <c r="B39" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="10">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="D39" s="27"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="6">
+        <f>1/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="F39" s="17"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
       <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="5"/>
       <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="29"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
       <c r="B41" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
       <c r="B42" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
       <c r="B43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
       <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
       <c r="B45" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
       <c r="B46" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
       <c r="B47" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
       <c r="B48" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
       <c r="B49" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
       <c r="B50" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
       <c r="B51" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
       <c r="B52" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="15"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="9">
+      <c r="E52" s="32"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="24"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="7">
         <f>12/12</f>
         <v>1</v>
       </c>
-      <c r="D53" s="19"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A53"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A3:A15"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrección casos de prueba
Se corrigieron y actualizaron los casos de prueba, Se agregaron algunos
pantallazos del funcionamiento de la aplicación
</commit_message>
<xml_diff>
--- a/Documentation/Diagnostico App.xlsx
+++ b/Documentation/Diagnostico App.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
   <si>
     <t>Login</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>El usuario debe conocer los codigos de los otros grupos?</t>
+  </si>
+  <si>
+    <t>Falta toast identificador</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -305,26 +308,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -398,98 +381,61 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,6 +452,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1121352</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>173181</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3679312</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>11689</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13053579" y="10927772"/>
+          <a:ext cx="3978051" cy="7077508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1176103</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>86589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>35019</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13108330" y="18270680"/>
+          <a:ext cx="3932761" cy="6996930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1204283</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>160252</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13129583" y="25488900"/>
+          <a:ext cx="4091617" cy="7246852"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -773,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="O96" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,30 +865,30 @@
     <col min="1" max="1" width="27.125" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="20" t="s">
+      <c r="D1" s="13"/>
+      <c r="E1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="21"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="3" t="s">
         <v>51</v>
       </c>
@@ -820,7 +903,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -832,7 +915,7 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -842,13 +925,13 @@
       <c r="D4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>52</v>
+      <c r="E4" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -858,13 +941,13 @@
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>52</v>
+      <c r="E5" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -874,13 +957,13 @@
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="6" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -890,13 +973,13 @@
       <c r="D7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>52</v>
+      <c r="E7" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
@@ -906,23 +989,23 @@
       <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="6" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="27"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
@@ -932,13 +1015,13 @@
       <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="27" t="s">
-        <v>52</v>
+      <c r="E10" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
@@ -948,13 +1031,13 @@
       <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>52</v>
+      <c r="E11" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
@@ -964,13 +1047,13 @@
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="6" t="s">
         <v>45</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
@@ -980,13 +1063,13 @@
       <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="27" t="s">
-        <v>52</v>
+      <c r="E13" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
       <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
@@ -996,29 +1079,28 @@
       <c r="D14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="6" t="s">
         <v>45</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="20">
         <f>2/10</f>
         <v>0.2</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="9">
-        <f>4/10</f>
-        <v>0.4</v>
-      </c>
-      <c r="F15" s="40"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="23">
+        <v>1</v>
+      </c>
+      <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1030,11 +1112,13 @@
       <c r="D16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="29"/>
+      <c r="E16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1042,11 +1126,13 @@
         <v>45</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="32"/>
+      <c r="E17" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1054,11 +1140,13 @@
         <v>45</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="32"/>
+      <c r="E18" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1066,24 +1154,29 @@
         <v>45</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="32"/>
+      <c r="E19" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="23">
         <f>4/4</f>
         <v>1</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="12"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23">
+        <f>4/4</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1095,11 +1188,13 @@
       <c r="D21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="29"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="E21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1107,24 +1202,29 @@
         <v>41</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="32"/>
+      <c r="E22" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="23">
         <f>2/2</f>
         <v>1</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="12"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="23">
+        <f>2/2</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="24"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1142,7 +1242,7 @@
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1156,7 +1256,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
@@ -1174,7 +1274,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
@@ -1188,7 +1288,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1201,8 +1301,8 @@
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
@@ -1216,22 +1316,22 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
-      <c r="B30" s="13" t="s">
+      <c r="A30" s="10"/>
+      <c r="B30" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="32">
         <f>5/6</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="7">
+      <c r="D30" s="33"/>
+      <c r="E30" s="23">
         <v>1</v>
       </c>
-      <c r="F30" s="28"/>
+      <c r="F30" s="25"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1241,11 +1341,13 @@
         <v>45</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
+      <c r="E31" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
       <c r="B32" s="1" t="s">
         <v>21</v>
       </c>
@@ -1255,24 +1357,30 @@
       <c r="D32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
+      <c r="E32" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24"/>
-      <c r="B33" s="14" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="27">
         <f>1/2</f>
         <v>0.5</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="38"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="29">
+        <v>1</v>
+      </c>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1281,10 +1389,10 @@
       <c r="C34" s="5"/>
       <c r="D34" s="2"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="29"/>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="1" t="s">
         <v>24</v>
       </c>
@@ -1302,7 +1410,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="1" t="s">
         <v>25</v>
       </c>
@@ -1320,7 +1428,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="1" t="s">
         <v>26</v>
       </c>
@@ -1337,8 +1445,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
+    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="9"/>
       <c r="B38" s="1" t="s">
         <v>27</v>
       </c>
@@ -1356,33 +1464,33 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="23"/>
-      <c r="B39" s="18" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="20">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="6">
+      <c r="D39" s="21"/>
+      <c r="E39" s="20">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" s="21"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="29"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="1" t="s">
         <v>29</v>
       </c>
@@ -1390,11 +1498,11 @@
         <v>41</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="32"/>
+      <c r="E41" s="5"/>
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="1" t="s">
         <v>30</v>
       </c>
@@ -1402,11 +1510,11 @@
         <v>41</v>
       </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="32"/>
+      <c r="E42" s="5"/>
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="1" t="s">
         <v>31</v>
       </c>
@@ -1414,11 +1522,11 @@
         <v>41</v>
       </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="32"/>
+      <c r="E43" s="5"/>
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
@@ -1426,11 +1534,11 @@
         <v>41</v>
       </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="32"/>
+      <c r="E44" s="5"/>
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="1" t="s">
         <v>33</v>
       </c>
@@ -1438,11 +1546,11 @@
         <v>41</v>
       </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="32"/>
+      <c r="E45" s="5"/>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="1" t="s">
         <v>34</v>
       </c>
@@ -1450,11 +1558,11 @@
         <v>41</v>
       </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="32"/>
+      <c r="E46" s="5"/>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="1" t="s">
         <v>35</v>
       </c>
@@ -1462,11 +1570,11 @@
         <v>41</v>
       </c>
       <c r="D47" s="2"/>
-      <c r="E47" s="32"/>
+      <c r="E47" s="5"/>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1474,11 +1582,11 @@
         <v>41</v>
       </c>
       <c r="D48" s="2"/>
-      <c r="E48" s="32"/>
+      <c r="E48" s="5"/>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="1" t="s">
         <v>37</v>
       </c>
@@ -1486,11 +1594,11 @@
         <v>41</v>
       </c>
       <c r="D49" s="2"/>
-      <c r="E49" s="32"/>
+      <c r="E49" s="5"/>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+      <c r="A50" s="9"/>
       <c r="B50" s="1" t="s">
         <v>38</v>
       </c>
@@ -1498,11 +1606,11 @@
         <v>41</v>
       </c>
       <c r="D50" s="2"/>
-      <c r="E50" s="32"/>
+      <c r="E50" s="5"/>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
+      <c r="A51" s="9"/>
       <c r="B51" s="1" t="s">
         <v>39</v>
       </c>
@@ -1510,11 +1618,11 @@
         <v>41</v>
       </c>
       <c r="D51" s="2"/>
-      <c r="E51" s="32"/>
+      <c r="E51" s="5"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
+    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
       <c r="B52" s="1" t="s">
         <v>40</v>
       </c>
@@ -1522,34 +1630,35 @@
         <v>41</v>
       </c>
       <c r="D52" s="2"/>
-      <c r="E52" s="32"/>
+      <c r="E52" s="5"/>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="24"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="7">
+      <c r="A53" s="10"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="23">
         <f>12/12</f>
         <v>1</v>
       </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="12"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A3:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A30"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A53"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A3:A15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A21:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se insertaron las pruebas de la entrega 3
Pruebas de la entrega 3 realizadas. Sin cambios
</commit_message>
<xml_diff>
--- a/Documentation/Diagnostico App.xlsx
+++ b/Documentation/Diagnostico App.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pruebas Sprint 3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="64">
   <si>
     <t>Login</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Falta toast identificador</t>
+  </si>
+  <si>
+    <t>Entrega 2</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -381,12 +384,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -396,27 +419,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -436,6 +438,33 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,15 +576,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1204283</xdr:colOff>
-      <xdr:row>133</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>1156659</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>171</xdr:row>
-      <xdr:rowOff>160252</xdr:rowOff>
+      <xdr:colOff>40340</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>184063</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -578,8 +607,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13129583" y="25488900"/>
-          <a:ext cx="4091617" cy="7246852"/>
+          <a:off x="13110534" y="25312686"/>
+          <a:ext cx="4003369" cy="7065877"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -854,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="O96" sqref="O96"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,27 +897,33 @@
     <col min="4" max="4" width="58.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="48.5" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="3" t="s">
         <v>51</v>
       </c>
@@ -901,9 +936,15 @@
       <c r="F2" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="G2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -913,9 +954,11 @@
       <c r="D3" s="2"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -929,9 +972,13 @@
         <v>45</v>
       </c>
       <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="G4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -945,9 +992,13 @@
         <v>45</v>
       </c>
       <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="G5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -961,9 +1012,13 @@
         <v>45</v>
       </c>
       <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="G6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -977,9 +1032,13 @@
         <v>45</v>
       </c>
       <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="G7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
       <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
@@ -993,9 +1052,13 @@
         <v>45</v>
       </c>
       <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="G8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
       <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1003,9 +1066,11 @@
       <c r="D9" s="2"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
       <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
@@ -1019,9 +1084,13 @@
         <v>45</v>
       </c>
       <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="G10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
@@ -1035,9 +1104,13 @@
         <v>45</v>
       </c>
       <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="G11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
       <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
@@ -1051,9 +1124,13 @@
         <v>45</v>
       </c>
       <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="G12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
       <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
@@ -1067,9 +1144,13 @@
         <v>45</v>
       </c>
       <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+      <c r="G13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="31"/>
       <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1083,24 +1164,32 @@
         <v>45</v>
       </c>
       <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="34" t="s">
+      <c r="G14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="32"/>
+      <c r="B15" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="13">
         <f>2/10</f>
         <v>0.2</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="23">
+      <c r="D15" s="14"/>
+      <c r="E15" s="16">
         <v>1</v>
       </c>
-      <c r="F15" s="25"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="F15" s="18"/>
+      <c r="G15" s="16">
+        <v>1</v>
+      </c>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1115,10 +1204,18 @@
       <c r="E16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="F16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1130,9 +1227,13 @@
         <v>45</v>
       </c>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="G17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1144,9 +1245,13 @@
         <v>45</v>
       </c>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
+      <c r="G18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33"/>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1158,25 +1263,34 @@
         <v>45</v>
       </c>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="22" t="s">
+      <c r="G19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34"/>
+      <c r="B20" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="16">
         <f>4/4</f>
         <v>1</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="23">
+      <c r="D20" s="17"/>
+      <c r="E20" s="16">
         <f>4/4</f>
         <v>1</v>
       </c>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="F20" s="17"/>
+      <c r="G20" s="16">
+        <f>4/4</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1192,9 +1306,13 @@
         <v>41</v>
       </c>
       <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
+      <c r="G21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1206,25 +1324,34 @@
         <v>41</v>
       </c>
       <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="22" t="s">
+      <c r="G22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="16">
         <f>2/2</f>
         <v>1</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="23">
+      <c r="D23" s="17"/>
+      <c r="E23" s="16">
         <f>2/2</f>
         <v>1</v>
       </c>
-      <c r="F23" s="24"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="F23" s="17"/>
+      <c r="G23" s="16">
+        <f>2/2</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1240,9 +1367,13 @@
         <v>41</v>
       </c>
       <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="G24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1254,9 +1385,13 @@
         <v>45</v>
       </c>
       <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="G25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
       <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
@@ -1272,9 +1407,15 @@
       <c r="F26" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="G26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
@@ -1286,9 +1427,13 @@
         <v>41</v>
       </c>
       <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="G27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1300,9 +1445,13 @@
         <v>41</v>
       </c>
       <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
+      <c r="G28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="31"/>
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
@@ -1314,24 +1463,32 @@
         <v>41</v>
       </c>
       <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="31" t="s">
+      <c r="G29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="32"/>
+      <c r="B30" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="25">
         <f>5/6</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="23">
+      <c r="D30" s="26"/>
+      <c r="E30" s="16">
         <v>1</v>
       </c>
-      <c r="F30" s="25"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="F30" s="18"/>
+      <c r="G30" s="16">
+        <v>1</v>
+      </c>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1341,13 +1498,17 @@
         <v>45</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="9" t="s">
         <v>45</v>
       </c>
       <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
+      <c r="G31" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="31"/>
       <c r="B32" s="1" t="s">
         <v>21</v>
       </c>
@@ -1357,30 +1518,40 @@
       <c r="D32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="18" t="s">
+      <c r="E32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
-      <c r="B33" s="26" t="s">
+      <c r="G32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="32"/>
+      <c r="B33" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="27">
+      <c r="C33" s="20">
         <f>1/2</f>
         <v>0.5</v>
       </c>
-      <c r="D33" s="28"/>
-      <c r="E33" s="29">
+      <c r="D33" s="21"/>
+      <c r="E33" s="22">
         <v>1</v>
       </c>
-      <c r="F33" s="30"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="F33" s="23"/>
+      <c r="G33" s="22">
+        <v>1</v>
+      </c>
+      <c r="H33" s="23"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1390,9 +1561,11 @@
       <c r="D34" s="2"/>
       <c r="E34" s="4"/>
       <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
       <c r="B35" s="1" t="s">
         <v>24</v>
       </c>
@@ -1408,9 +1581,15 @@
       <c r="F35" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
+      <c r="G35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
       <c r="B36" s="1" t="s">
         <v>25</v>
       </c>
@@ -1426,9 +1605,15 @@
       <c r="F36" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
+      <c r="G36" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
       <c r="B37" s="1" t="s">
         <v>26</v>
       </c>
@@ -1444,9 +1629,15 @@
       <c r="F37" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
+      <c r="G37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="31"/>
       <c r="B38" s="1" t="s">
         <v>27</v>
       </c>
@@ -1462,25 +1653,36 @@
       <c r="F38" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
-      <c r="B39" s="19" t="s">
+      <c r="G38" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="31"/>
+      <c r="B39" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C39" s="13">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="20">
+      <c r="D39" s="14"/>
+      <c r="E39" s="13">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="F39" s="21"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="13">
+        <f>1/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="H39" s="14"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
       <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
@@ -1488,9 +1690,11 @@
       <c r="D40" s="2"/>
       <c r="E40" s="4"/>
       <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
       <c r="B41" s="1" t="s">
         <v>29</v>
       </c>
@@ -1500,9 +1704,11 @@
       <c r="D41" s="2"/>
       <c r="E41" s="5"/>
       <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
       <c r="B42" s="1" t="s">
         <v>30</v>
       </c>
@@ -1512,9 +1718,11 @@
       <c r="D42" s="2"/>
       <c r="E42" s="5"/>
       <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
       <c r="B43" s="1" t="s">
         <v>31</v>
       </c>
@@ -1524,9 +1732,11 @@
       <c r="D43" s="2"/>
       <c r="E43" s="5"/>
       <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
       <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
@@ -1536,9 +1746,11 @@
       <c r="D44" s="2"/>
       <c r="E44" s="5"/>
       <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="31"/>
       <c r="B45" s="1" t="s">
         <v>33</v>
       </c>
@@ -1548,9 +1760,11 @@
       <c r="D45" s="2"/>
       <c r="E45" s="5"/>
       <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="31"/>
       <c r="B46" s="1" t="s">
         <v>34</v>
       </c>
@@ -1560,9 +1774,11 @@
       <c r="D46" s="2"/>
       <c r="E46" s="5"/>
       <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
       <c r="B47" s="1" t="s">
         <v>35</v>
       </c>
@@ -1572,9 +1788,11 @@
       <c r="D47" s="2"/>
       <c r="E47" s="5"/>
       <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
       <c r="B48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1584,9 +1802,11 @@
       <c r="D48" s="2"/>
       <c r="E48" s="5"/>
       <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="31"/>
       <c r="B49" s="1" t="s">
         <v>37</v>
       </c>
@@ -1596,9 +1816,11 @@
       <c r="D49" s="2"/>
       <c r="E49" s="5"/>
       <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="31"/>
       <c r="B50" s="1" t="s">
         <v>38</v>
       </c>
@@ -1608,9 +1830,11 @@
       <c r="D50" s="2"/>
       <c r="E50" s="5"/>
       <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="31"/>
       <c r="B51" s="1" t="s">
         <v>39</v>
       </c>
@@ -1620,9 +1844,11 @@
       <c r="D51" s="2"/>
       <c r="E51" s="5"/>
       <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="31"/>
       <c r="B52" s="1" t="s">
         <v>40</v>
       </c>
@@ -1632,30 +1858,35 @@
       <c r="D52" s="2"/>
       <c r="E52" s="5"/>
       <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="23">
+      <c r="G52" s="5"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="32"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="16">
         <f>12/12</f>
         <v>1</v>
       </c>
-      <c r="D53" s="24"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="24"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A53"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A3:A15"/>
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>